<commit_message>
feat: Add Sector ETF support, optimize data update, and fix UI/ticker bugs
</commit_message>
<xml_diff>
--- a/etf_list.xlsx
+++ b/etf_list.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdk72\Documents\project\ETF_주도주전략_rev1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B154638A-0452-44E7-B420-9AA8913F21A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79975F0A-0EB1-44B5-8831-46E2F1A39CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EB69685F-6182-49E3-90FF-80D8DF2A9EC2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EB69685F-6182-49E3-90FF-80D8DF2A9EC2}"/>
   </bookViews>
   <sheets>
-    <sheet name="93종목" sheetId="1" r:id="rId1"/>
+    <sheet name="테마etf_list" sheetId="1" r:id="rId1"/>
+    <sheet name="섹터etf_list" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="221">
   <si>
     <t>종목명</t>
   </si>
@@ -375,6 +376,330 @@
   </si>
   <si>
     <t>HANARO Fn골프테마</t>
+  </si>
+  <si>
+    <t>TIGER 반도체TOP10</t>
+  </si>
+  <si>
+    <t>KODEX 반도체</t>
+  </si>
+  <si>
+    <t>SOL 조선TOP3플러스</t>
+  </si>
+  <si>
+    <t>KODEX AI반도체</t>
+  </si>
+  <si>
+    <t>TIGER 조선TOP10</t>
+  </si>
+  <si>
+    <t>HANARO Fn K-반도체</t>
+  </si>
+  <si>
+    <t>TIGER 200 IT</t>
+  </si>
+  <si>
+    <t>TIGER 반도체</t>
+  </si>
+  <si>
+    <t>SOL AI반도체소부장</t>
+  </si>
+  <si>
+    <t>KoAct 바이오헬스케어액티브</t>
+  </si>
+  <si>
+    <t>TIMEFOLIO K바이오액티브</t>
+  </si>
+  <si>
+    <t>KODEX 은행</t>
+  </si>
+  <si>
+    <t>KODEX 증권</t>
+  </si>
+  <si>
+    <t>KODEX 자동차</t>
+  </si>
+  <si>
+    <t>TIGER 200 중공업</t>
+  </si>
+  <si>
+    <t>TIGER 코리아AI전력기기TOP3플러스</t>
+  </si>
+  <si>
+    <t>TIGER 화장품</t>
+  </si>
+  <si>
+    <t>TIGER 바이오TOP10</t>
+  </si>
+  <si>
+    <t>RISE AI&amp;로봇</t>
+  </si>
+  <si>
+    <t>KODEX 바이오</t>
+  </si>
+  <si>
+    <t>TIGER 헬스케어</t>
+  </si>
+  <si>
+    <t>KODEX AI반도체핵심장비</t>
+  </si>
+  <si>
+    <t>RISE 비메모리반도체액티브</t>
+  </si>
+  <si>
+    <t>KODEX K방산TOP10</t>
+  </si>
+  <si>
+    <t>ACE AI반도체포커스</t>
+  </si>
+  <si>
+    <t>TIGER 소프트웨어</t>
+  </si>
+  <si>
+    <t>TIGER 증권</t>
+  </si>
+  <si>
+    <t>TIGER 미디어컨텐츠</t>
+  </si>
+  <si>
+    <t>SOL 자동차TOP3플러스</t>
+  </si>
+  <si>
+    <t>KODEX 코리아소버린AI</t>
+  </si>
+  <si>
+    <t>WON 반도체밸류체인액티브</t>
+  </si>
+  <si>
+    <t>HANARO Fn조선해운</t>
+  </si>
+  <si>
+    <t>KODEX 헬스케어</t>
+  </si>
+  <si>
+    <t>TIGER AI반도체핵심공정</t>
+  </si>
+  <si>
+    <t>RISE 메타버스</t>
+  </si>
+  <si>
+    <t>TIGER 여행레저</t>
+  </si>
+  <si>
+    <t>KODEX K조선TOP10</t>
+  </si>
+  <si>
+    <t>SOL 화장품TOP3플러스</t>
+  </si>
+  <si>
+    <t>SOL K방산</t>
+  </si>
+  <si>
+    <t>RISE 네트워크인프라</t>
+  </si>
+  <si>
+    <t>KODEX 메타버스액티브</t>
+  </si>
+  <si>
+    <t>HANARO CAPEX설비투자iSelect</t>
+  </si>
+  <si>
+    <t>RISE IT플러스</t>
+  </si>
+  <si>
+    <t>KODEX 200IT TR</t>
+  </si>
+  <si>
+    <t>HANARO 전력설비투자</t>
+  </si>
+  <si>
+    <t>UNICORN SK하이닉스밸류체인액티브</t>
+  </si>
+  <si>
+    <t>현대자산운용</t>
+  </si>
+  <si>
+    <t>TIGER 인터넷TOP10</t>
+  </si>
+  <si>
+    <t>HANARO Fn K-POP&amp;미디어</t>
+  </si>
+  <si>
+    <t>TIGER Fn메타버스</t>
+  </si>
+  <si>
+    <t>TIGER 경기방어</t>
+  </si>
+  <si>
+    <t>RISE AI전력인프라</t>
+  </si>
+  <si>
+    <t>TIGER 게임TOP10</t>
+  </si>
+  <si>
+    <t>KODEX K콘텐츠</t>
+  </si>
+  <si>
+    <t>KODEX 보험</t>
+  </si>
+  <si>
+    <t>RISE AI반도체TOP10</t>
+  </si>
+  <si>
+    <t>RISE 바이오TOP10액티브</t>
+  </si>
+  <si>
+    <t>SOL 반도체전공정</t>
+  </si>
+  <si>
+    <t>KODEX IT</t>
+  </si>
+  <si>
+    <t>HANARO 증권고배당TOP3플러스</t>
+  </si>
+  <si>
+    <t>TIGER 200 헬스케어</t>
+  </si>
+  <si>
+    <t>KODEX 건설</t>
+  </si>
+  <si>
+    <t>BNK 온디바이스AI</t>
+  </si>
+  <si>
+    <t>1Q K소버린AI</t>
+  </si>
+  <si>
+    <t>TIGER 200 금융</t>
+  </si>
+  <si>
+    <t>KODEX 에너지화학</t>
+  </si>
+  <si>
+    <t>TIGER 200 건설</t>
+  </si>
+  <si>
+    <t>SOL 반도체후공정</t>
+  </si>
+  <si>
+    <t>RISE 내수주플러스</t>
+  </si>
+  <si>
+    <t>TIGER 200 에너지화학</t>
+  </si>
+  <si>
+    <t>ITF K-AI반도체코어테크</t>
+  </si>
+  <si>
+    <t>아이비케이자산운용</t>
+  </si>
+  <si>
+    <t>TIGER 한중반도체(합성)</t>
+  </si>
+  <si>
+    <t>KODEX 철강</t>
+  </si>
+  <si>
+    <t>PLUS K방산레버리지</t>
+  </si>
+  <si>
+    <t>KODEX 기계장비</t>
+  </si>
+  <si>
+    <t>TIGER 코리아휴머노이드로봇산업</t>
+  </si>
+  <si>
+    <t>HANARO Fn K-푸드</t>
+  </si>
+  <si>
+    <t>KODEX 한중반도체(합성)</t>
+  </si>
+  <si>
+    <t>SOL 한국AI소프트웨어</t>
+  </si>
+  <si>
+    <t>HANARO 바이오코리아액티브</t>
+  </si>
+  <si>
+    <t>SOL 조선기자재</t>
+  </si>
+  <si>
+    <t>RISE 200금융</t>
+  </si>
+  <si>
+    <t>KIWOOM K-테크TOP10</t>
+  </si>
+  <si>
+    <t>TIGER 은행</t>
+  </si>
+  <si>
+    <t>SOL 의료기기소부장Fn</t>
+  </si>
+  <si>
+    <t>마이티 바이오시밀러&amp;CDMO액티브</t>
+  </si>
+  <si>
+    <t>DB자산운용</t>
+  </si>
+  <si>
+    <t>KODEX 운송</t>
+  </si>
+  <si>
+    <t>PLUS K방산소부장</t>
+  </si>
+  <si>
+    <t>KODEX 필수소비재</t>
+  </si>
+  <si>
+    <t>HANARO Fn5G산업</t>
+  </si>
+  <si>
+    <t>SOL 자동차소부장Fn</t>
+  </si>
+  <si>
+    <t>HANARO Fn K-게임</t>
+  </si>
+  <si>
+    <t>HANARO 반도체핵심공정주도주</t>
+  </si>
+  <si>
+    <t>RISE 헬스케어</t>
+  </si>
+  <si>
+    <t>TIGER 의료기기</t>
+  </si>
+  <si>
+    <t>KIWOOM 의료AI</t>
+  </si>
+  <si>
+    <t>ACE 코리아AI테크핵심산업</t>
+  </si>
+  <si>
+    <t>TIGER 200 산업재</t>
+  </si>
+  <si>
+    <t>TIGER 200 경기소비재</t>
+  </si>
+  <si>
+    <t>TIGER 200 철강소재</t>
+  </si>
+  <si>
+    <t>KIWOOM Fn유전자혁신기술</t>
+  </si>
+  <si>
+    <t>KODEX 경기소비재</t>
+  </si>
+  <si>
+    <t>HANARO Fn K-메타버스MZ</t>
+  </si>
+  <si>
+    <t>TIGER 200 생활소비재</t>
+  </si>
+  <si>
+    <t>KIWOOM K-반도체북미공급망</t>
+  </si>
+  <si>
+    <t>UNICORN 생성형AI강소기업액티브</t>
   </si>
 </sst>
 </file>
@@ -450,7 +775,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -458,6 +783,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -796,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0A8663-262E-4D49-9E4F-7F90AF409F72}">
   <dimension ref="A1:B94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1558,4 +1892,870 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC065381-1176-4F66-A90C-28D6B9B9266C}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:B106"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B106"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B61" s="5"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B91" s="5"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>